<commit_message>
Join with extend implemented
</commit_message>
<xml_diff>
--- a/test/Test1.xlsx
+++ b/test/Test1.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="hssv4XbWexGpTebjvWKdz/ZoDJAxuYABNzgqQj+8E1E="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="UB94c6XuKsBIWHcbdLLL0/+hhs5krEtBeoZqUgZv+00="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>Organization</t>
   </si>
@@ -24,7 +24,8 @@
     <t>Optional age</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Name
+Multiline</t>
   </si>
   <si>
     <t>Team</t>
@@ -127,36 +128,6 @@
   </si>
   <si>
     <t>Orlando Wright</t>
-  </si>
-  <si>
-    <t>Amira Kerr [C]</t>
-  </si>
-  <si>
-    <t>Platform and application</t>
-  </si>
-  <si>
-    <t>Jayleen Larsen</t>
-  </si>
-  <si>
-    <t>Britney Peterson</t>
-  </si>
-  <si>
-    <t>Luke Holloway (On Leave)</t>
-  </si>
-  <si>
-    <t>Mathew Alexander</t>
-  </si>
-  <si>
-    <t>PIC design</t>
-  </si>
-  <si>
-    <t>Frank Lindsey</t>
-  </si>
-  <si>
-    <t>OEQ</t>
-  </si>
-  <si>
-    <t>Miss Outsideorg</t>
   </si>
 </sst>
 </file>
@@ -441,7 +412,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -729,95 +700,89 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+    </row>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -1779,6 +1744,13 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>